<commit_message>
MISE A JOUR DU BACKLOG
</commit_message>
<xml_diff>
--- a/TachesEDT.xlsx
+++ b/TachesEDT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="106">
   <si>
     <t>Page</t>
   </si>
@@ -362,7 +362,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -442,6 +442,13 @@
       <b/>
       <sz val="14"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -575,7 +582,7 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -659,9 +666,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -697,35 +701,60 @@
     <xf numFmtId="14" fontId="4" fillId="4" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1036,8 +1065,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K46" sqref="K46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1080,20 +1109,20 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="36"/>
+      <c r="A2" s="35"/>
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
       <c r="D2" s="11"/>
-      <c r="E2" s="33"/>
+      <c r="E2" s="32"/>
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
       <c r="H2" s="10"/>
     </row>
     <row r="3" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="43" t="s">
+      <c r="B3" s="51" t="s">
         <v>14</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -1102,7 +1131,7 @@
       <c r="D3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="35" t="s">
+      <c r="E3" s="34" t="s">
         <v>73</v>
       </c>
       <c r="F3" s="27"/>
@@ -1112,15 +1141,15 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="46"/>
-      <c r="B4" s="43"/>
+      <c r="A4" s="43"/>
+      <c r="B4" s="51"/>
       <c r="C4" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="35" t="s">
+      <c r="E4" s="34" t="s">
         <v>73</v>
       </c>
       <c r="F4" s="27"/>
@@ -1130,15 +1159,15 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="46"/>
-      <c r="B5" s="43"/>
+      <c r="A5" s="43"/>
+      <c r="B5" s="51"/>
       <c r="C5" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="E5" s="35" t="s">
+      <c r="E5" s="34" t="s">
         <v>73</v>
       </c>
       <c r="F5" s="27"/>
@@ -1148,15 +1177,15 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="46"/>
-      <c r="B6" s="43"/>
+      <c r="A6" s="43"/>
+      <c r="B6" s="51"/>
       <c r="C6" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="35" t="s">
+      <c r="E6" s="34" t="s">
         <v>73</v>
       </c>
       <c r="F6" s="27"/>
@@ -1166,7 +1195,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="47"/>
+      <c r="A7" s="44"/>
       <c r="B7" s="4" t="s">
         <v>15</v>
       </c>
@@ -1176,7 +1205,7 @@
       <c r="D7" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="35" t="s">
+      <c r="E7" s="34" t="s">
         <v>73</v>
       </c>
       <c r="F7" s="27"/>
@@ -1186,10 +1215,10 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="45" t="s">
+      <c r="A8" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="51" t="s">
         <v>19</v>
       </c>
       <c r="C8" s="16" t="s">
@@ -1198,7 +1227,7 @@
       <c r="D8" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="30" t="s">
+      <c r="E8" s="29" t="s">
         <v>74</v>
       </c>
       <c r="F8" s="27"/>
@@ -1208,15 +1237,15 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="46"/>
-      <c r="B9" s="43"/>
+      <c r="A9" s="43"/>
+      <c r="B9" s="51"/>
       <c r="C9" s="15" t="s">
         <v>48</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="30" t="s">
+      <c r="E9" s="29" t="s">
         <v>74</v>
       </c>
       <c r="F9" s="27"/>
@@ -1226,15 +1255,15 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="46"/>
-      <c r="B10" s="43"/>
+      <c r="A10" s="43"/>
+      <c r="B10" s="51"/>
       <c r="C10" s="15" t="s">
         <v>20</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E10" s="30" t="s">
+      <c r="E10" s="29" t="s">
         <v>74</v>
       </c>
       <c r="F10" s="27"/>
@@ -1244,15 +1273,15 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="46"/>
-      <c r="B11" s="43"/>
+      <c r="A11" s="43"/>
+      <c r="B11" s="51"/>
       <c r="C11" s="16" t="s">
         <v>21</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="30" t="s">
+      <c r="E11" s="29" t="s">
         <v>74</v>
       </c>
       <c r="F11" s="27"/>
@@ -1260,21 +1289,21 @@
       <c r="H11" s="15"/>
     </row>
     <row r="12" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="46"/>
-      <c r="B12" s="43" t="s">
+      <c r="A12" s="43"/>
+      <c r="B12" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="40" t="s">
+      <c r="C12" s="39" t="s">
         <v>53</v>
       </c>
-      <c r="D12" s="38" t="s">
+      <c r="D12" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="E12" s="31" t="s">
+      <c r="E12" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="F12" s="41"/>
-      <c r="G12" s="42">
+      <c r="F12" s="40"/>
+      <c r="G12" s="41">
         <v>41429</v>
       </c>
       <c r="H12" s="23" t="s">
@@ -1282,19 +1311,19 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="46"/>
-      <c r="B13" s="43"/>
-      <c r="C13" s="40" t="s">
+      <c r="A13" s="43"/>
+      <c r="B13" s="51"/>
+      <c r="C13" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="D13" s="38" t="s">
+      <c r="D13" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="31" t="s">
+      <c r="E13" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="F13" s="41"/>
-      <c r="G13" s="42">
+      <c r="F13" s="40"/>
+      <c r="G13" s="41">
         <v>41429</v>
       </c>
       <c r="H13" s="23" t="s">
@@ -1302,15 +1331,15 @@
       </c>
     </row>
     <row r="14" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="46"/>
-      <c r="B14" s="43"/>
+      <c r="A14" s="43"/>
+      <c r="B14" s="51"/>
       <c r="C14" s="16" t="s">
         <v>27</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E14" s="30" t="s">
+      <c r="E14" s="29" t="s">
         <v>74</v>
       </c>
       <c r="F14" s="27"/>
@@ -1320,8 +1349,8 @@
       </c>
     </row>
     <row r="15" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="46"/>
-      <c r="B15" s="44" t="s">
+      <c r="A15" s="43"/>
+      <c r="B15" s="50" t="s">
         <v>30</v>
       </c>
       <c r="C15" s="16" t="s">
@@ -1330,7 +1359,7 @@
       <c r="D15" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="30" t="s">
+      <c r="E15" s="29" t="s">
         <v>74</v>
       </c>
       <c r="F15" s="27"/>
@@ -1340,15 +1369,15 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="46"/>
-      <c r="B16" s="44"/>
+      <c r="A16" s="43"/>
+      <c r="B16" s="50"/>
       <c r="C16" s="15" t="s">
         <v>50</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E16" s="30" t="s">
+      <c r="E16" s="29" t="s">
         <v>74</v>
       </c>
       <c r="F16" s="27"/>
@@ -1358,15 +1387,15 @@
       </c>
     </row>
     <row r="17" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="46"/>
-      <c r="B17" s="44"/>
+      <c r="A17" s="43"/>
+      <c r="B17" s="50"/>
       <c r="C17" s="15" t="s">
         <v>31</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E17" s="30" t="s">
+      <c r="E17" s="29" t="s">
         <v>74</v>
       </c>
       <c r="F17" s="27"/>
@@ -1376,7 +1405,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="46"/>
+      <c r="A18" s="43"/>
       <c r="B18" s="16" t="s">
         <v>35</v>
       </c>
@@ -1386,7 +1415,7 @@
       <c r="D18" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="E18" s="30" t="s">
+      <c r="E18" s="29" t="s">
         <v>74</v>
       </c>
       <c r="F18" s="27"/>
@@ -1396,8 +1425,8 @@
       </c>
     </row>
     <row r="19" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="46"/>
-      <c r="B19" s="44" t="s">
+      <c r="A19" s="43"/>
+      <c r="B19" s="50" t="s">
         <v>38</v>
       </c>
       <c r="C19" s="16" t="s">
@@ -1406,7 +1435,7 @@
       <c r="D19" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E19" s="30" t="s">
+      <c r="E19" s="29" t="s">
         <v>74</v>
       </c>
       <c r="F19" s="27"/>
@@ -1416,15 +1445,15 @@
       </c>
     </row>
     <row r="20" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="46"/>
-      <c r="B20" s="44"/>
+      <c r="A20" s="43"/>
+      <c r="B20" s="50"/>
       <c r="C20" s="16" t="s">
         <v>40</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E20" s="30" t="s">
+      <c r="E20" s="29" t="s">
         <v>74</v>
       </c>
       <c r="F20" s="27"/>
@@ -1434,19 +1463,19 @@
       </c>
     </row>
     <row r="21" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="46"/>
-      <c r="B21" s="44"/>
-      <c r="C21" s="51" t="s">
+      <c r="A21" s="43"/>
+      <c r="B21" s="50"/>
+      <c r="C21" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="52"/>
-      <c r="E21" s="32"/>
+      <c r="D21" s="49"/>
+      <c r="E21" s="31"/>
       <c r="F21" s="27"/>
       <c r="G21" s="26"/>
       <c r="H21" s="15"/>
     </row>
     <row r="22" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="47"/>
+      <c r="A22" s="44"/>
       <c r="B22" s="15" t="s">
         <v>60</v>
       </c>
@@ -1456,7 +1485,7 @@
       <c r="D22" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="E22" s="30" t="s">
+      <c r="E22" s="29" t="s">
         <v>74</v>
       </c>
       <c r="F22" s="27"/>
@@ -1476,7 +1505,7 @@
       <c r="D23" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="E23" s="30" t="s">
+      <c r="E23" s="29" t="s">
         <v>74</v>
       </c>
       <c r="F23" s="27"/>
@@ -1496,7 +1525,7 @@
       <c r="D24" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="E24" s="30" t="s">
+      <c r="E24" s="29" t="s">
         <v>74</v>
       </c>
       <c r="F24" s="27"/>
@@ -1516,7 +1545,7 @@
       <c r="D25" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="E25" s="30" t="s">
+      <c r="E25" s="29" t="s">
         <v>74</v>
       </c>
       <c r="F25" s="27"/>
@@ -1536,7 +1565,7 @@
       <c r="D26" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="E26" s="30" t="s">
+      <c r="E26" s="29" t="s">
         <v>74</v>
       </c>
       <c r="F26" s="27"/>
@@ -1550,7 +1579,7 @@
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
       <c r="D27" s="11"/>
-      <c r="E27" s="33"/>
+      <c r="E27" s="32"/>
       <c r="F27" s="10"/>
       <c r="G27" s="10"/>
       <c r="H27" s="10"/>
@@ -1559,24 +1588,26 @@
       <c r="A28" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="B28" s="9" t="s">
+      <c r="B28" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="C28" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="D28" s="9" t="s">
+      <c r="D28" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="E28"/>
-      <c r="F28" s="27"/>
-      <c r="G28" s="26"/>
-      <c r="H28" s="9" t="s">
+      <c r="E28" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="F28" s="40"/>
+      <c r="G28" s="60"/>
+      <c r="H28" s="23" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="45" t="s">
+      <c r="A29" s="42" t="s">
         <v>86</v>
       </c>
       <c r="B29" s="12" t="s">
@@ -1589,7 +1620,7 @@
         <v>56</v>
       </c>
       <c r="E29" s="34" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F29" s="25"/>
       <c r="G29" s="9"/>
@@ -1598,21 +1629,21 @@
       </c>
     </row>
     <row r="30" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="46"/>
-      <c r="B30" s="48" t="s">
+      <c r="A30" s="43"/>
+      <c r="B30" s="45" t="s">
         <v>64</v>
       </c>
       <c r="C30" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="D30" s="37" t="s">
+      <c r="D30" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="E30" s="31" t="s">
+      <c r="E30" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="F30" s="41"/>
-      <c r="G30" s="42">
+      <c r="F30" s="40"/>
+      <c r="G30" s="41">
         <v>41429</v>
       </c>
       <c r="H30" s="23" t="s">
@@ -1620,19 +1651,19 @@
       </c>
     </row>
     <row r="31" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="46"/>
-      <c r="B31" s="49"/>
+      <c r="A31" s="43"/>
+      <c r="B31" s="46"/>
       <c r="C31" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="D31" s="38" t="s">
+      <c r="D31" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="E31" s="31" t="s">
+      <c r="E31" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="F31" s="41"/>
-      <c r="G31" s="42">
+      <c r="F31" s="40"/>
+      <c r="G31" s="41">
         <v>41429</v>
       </c>
       <c r="H31" s="23" t="s">
@@ -1640,19 +1671,19 @@
       </c>
     </row>
     <row r="32" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="46"/>
-      <c r="B32" s="50"/>
+      <c r="A32" s="43"/>
+      <c r="B32" s="47"/>
       <c r="C32" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="D32" s="39" t="s">
+      <c r="D32" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="E32" s="31" t="s">
+      <c r="E32" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="F32" s="41"/>
-      <c r="G32" s="42">
+      <c r="F32" s="40"/>
+      <c r="G32" s="41">
         <v>41429</v>
       </c>
       <c r="H32" s="23" t="s">
@@ -1660,7 +1691,7 @@
       </c>
     </row>
     <row r="33" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="46"/>
+      <c r="A33" s="43"/>
       <c r="B33" s="19" t="s">
         <v>75</v>
       </c>
@@ -1670,7 +1701,7 @@
       <c r="D33" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="E33" s="35" t="s">
+      <c r="E33" s="34" t="s">
         <v>73</v>
       </c>
       <c r="F33" s="27"/>
@@ -1680,27 +1711,29 @@
       </c>
     </row>
     <row r="34" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="46"/>
-      <c r="B34" s="19" t="s">
+      <c r="A34" s="43"/>
+      <c r="B34" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="C34" s="19" t="s">
+      <c r="C34" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="D34" s="6" t="s">
+      <c r="D34" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="E34" s="34" t="s">
-        <v>74</v>
-      </c>
-      <c r="F34" s="27"/>
-      <c r="G34" s="19"/>
-      <c r="H34" s="19" t="s">
+      <c r="E34" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="F34" s="40"/>
+      <c r="G34" s="58">
+        <v>41430</v>
+      </c>
+      <c r="H34" s="23" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="47"/>
+      <c r="A35" s="44"/>
       <c r="B35" s="19" t="s">
         <v>82</v>
       </c>
@@ -1710,7 +1743,7 @@
       <c r="D35" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="E35" s="34" t="s">
+      <c r="E35" s="33" t="s">
         <v>74</v>
       </c>
       <c r="F35" s="27"/>
@@ -1720,75 +1753,75 @@
       </c>
     </row>
     <row r="36" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="45" t="s">
+      <c r="A36" s="42" t="s">
         <v>85</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="53" t="s">
         <v>19</v>
       </c>
-      <c r="C36" s="20" t="s">
+      <c r="C36" s="54" t="s">
         <v>88</v>
       </c>
-      <c r="D36" s="6" t="s">
+      <c r="D36" s="55" t="s">
         <v>92</v>
       </c>
       <c r="E36" s="34" t="s">
-        <v>74</v>
-      </c>
-      <c r="F36" s="27"/>
-      <c r="G36" s="19"/>
-      <c r="H36" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="F36" s="59"/>
+      <c r="G36" s="52"/>
+      <c r="H36" s="52" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="46"/>
-      <c r="B37" s="4" t="s">
+      <c r="A37" s="43"/>
+      <c r="B37" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="C37" s="20" t="s">
+      <c r="C37" s="54" t="s">
         <v>87</v>
       </c>
-      <c r="D37" s="6" t="s">
+      <c r="D37" s="55" t="s">
         <v>93</v>
       </c>
       <c r="E37" s="34" t="s">
-        <v>74</v>
-      </c>
-      <c r="F37" s="27"/>
-      <c r="G37" s="19"/>
-      <c r="H37" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="F37" s="59"/>
+      <c r="G37" s="52"/>
+      <c r="H37" s="52" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="46"/>
-      <c r="B38" s="29" t="s">
+      <c r="A38" s="43"/>
+      <c r="B38" s="56" t="s">
         <v>30</v>
       </c>
-      <c r="C38" s="20" t="s">
+      <c r="C38" s="54" t="s">
         <v>89</v>
       </c>
-      <c r="D38" s="6" t="s">
+      <c r="D38" s="55" t="s">
         <v>94</v>
       </c>
       <c r="E38" s="34" t="s">
-        <v>74</v>
-      </c>
-      <c r="F38" s="27"/>
-      <c r="G38" s="19"/>
-      <c r="H38" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="F38" s="59"/>
+      <c r="G38" s="52"/>
+      <c r="H38" s="52" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="46"/>
+      <c r="A39" s="43"/>
       <c r="B39" s="20" t="s">
         <v>35</v>
       </c>
       <c r="C39" s="20"/>
       <c r="D39" s="6"/>
-      <c r="E39" s="34" t="s">
+      <c r="E39" s="33" t="s">
         <v>74</v>
       </c>
       <c r="F39" s="27"/>
@@ -1798,58 +1831,58 @@
       </c>
     </row>
     <row r="40" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="46"/>
-      <c r="B40" s="29" t="s">
+      <c r="A40" s="43"/>
+      <c r="B40" s="56" t="s">
         <v>38</v>
       </c>
-      <c r="C40" s="20" t="s">
+      <c r="C40" s="54" t="s">
         <v>90</v>
       </c>
-      <c r="D40" s="6" t="s">
+      <c r="D40" s="55" t="s">
         <v>95</v>
       </c>
       <c r="E40" s="34" t="s">
-        <v>74</v>
-      </c>
-      <c r="F40" s="27"/>
-      <c r="G40" s="19"/>
-      <c r="H40" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="F40" s="59"/>
+      <c r="G40" s="52"/>
+      <c r="H40" s="52" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="47"/>
-      <c r="B41" s="19" t="s">
+      <c r="A41" s="44"/>
+      <c r="B41" s="57" t="s">
         <v>60</v>
       </c>
-      <c r="C41" s="20" t="s">
+      <c r="C41" s="54" t="s">
         <v>91</v>
       </c>
-      <c r="D41" s="6" t="s">
+      <c r="D41" s="55" t="s">
         <v>96</v>
       </c>
       <c r="E41" s="34" t="s">
-        <v>74</v>
-      </c>
-      <c r="F41" s="27"/>
-      <c r="G41" s="19"/>
-      <c r="H41" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="F41" s="59"/>
+      <c r="G41" s="52"/>
+      <c r="H41" s="52" t="s">
         <v>51</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A29:A35"/>
-    <mergeCell ref="A36:A41"/>
-    <mergeCell ref="B30:B32"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="B19:B21"/>
     <mergeCell ref="B3:B6"/>
     <mergeCell ref="B8:B11"/>
     <mergeCell ref="B12:B14"/>
     <mergeCell ref="B15:B17"/>
     <mergeCell ref="A8:A22"/>
     <mergeCell ref="A3:A7"/>
+    <mergeCell ref="A29:A35"/>
+    <mergeCell ref="A36:A41"/>
+    <mergeCell ref="B30:B32"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="B19:B21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>